<commit_message>
fix : to_excel print 삭제
</commit_message>
<xml_diff>
--- a/data/excel/RecruitmentNotice.xlsx
+++ b/data/excel/RecruitmentNotice.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +595,60 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>(주)디셈버앤컴퍼니</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>핀트(fint) 프론트엔드(front-end) 개발자</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.jobplanet.co.kr/job/search?posting_ids%5B%5D=1290918</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>경력</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>react,typescript,jotai,emotion,webpack,babel,vue,angular</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>(주)버즈빌</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>[광고 추천팀] 백엔드 개발자 (Engineering Manager, Team Lead)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.jobplanet.co.kr/job/search?posting_ids%5B%5D=1288726</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>경력</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>go,python,mysql,dynamodb,redis,elasticsearch,kafka,kubernetes,grpc,apache,prometheus,kubernetes,spinnaker,datadog,grafana,prometheus,loki,aws,gcp</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix : SAMPLE_LIST 생성
</commit_message>
<xml_diff>
--- a/data/excel/RecruitmentNotice.xlsx
+++ b/data/excel/RecruitmentNotice.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -649,6 +649,83 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>(주)코그넷나인</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>프론트엔드개발자</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.jobplanet.co.kr/job/search?posting_ids%5B%5D=1290844</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>경력</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>react</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>(주)앤씨앤</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Embedded Application 개발자 채용</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.jobplanet.co.kr/job/search?posting_ids%5B%5D=1290660</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>경력</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>(주)유진로봇</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>개발본부 AMS팀 백엔드(Back-end) 개발자</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.jobplanet.co.kr/job/search?posting_ids%5B%5D=1269944</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>경력</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>javascript</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>